<commit_message>
Added electrical characterization plotting/
</commit_message>
<xml_diff>
--- a/Test_Data/1-23/results/Modeled power plot.xlsx
+++ b/Test_Data/1-23/results/Modeled power plot.xlsx
@@ -414,19 +414,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>23.94179623396392</v>
+        <v>24.24049683219419</v>
       </c>
       <c r="C2">
-        <v>57.2487654967684</v>
+        <v>58.37224775547493</v>
       </c>
       <c r="D2">
-        <v>228.8701403995201</v>
+        <v>249.2907120441463</v>
       </c>
       <c r="E2">
-        <v>72.98198442030836</v>
+        <v>84.54063340776146</v>
       </c>
       <c r="F2">
-        <v>2.554083663978645</v>
+        <v>2.58251337832879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected PV Flow rate miscalculation. Changed to instantaneous flow rate for calculating power. Added data smoothing to powerplot.
</commit_message>
<xml_diff>
--- a/Test_Data/1-23/results/Modeled power plot.xlsx
+++ b/Test_Data/1-23/results/Modeled power plot.xlsx
@@ -414,10 +414,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>24.24049683219419</v>
+        <v>16.52761147649603</v>
       </c>
       <c r="C2">
-        <v>58.37224775547493</v>
+        <v>66.80163065787728</v>
       </c>
       <c r="D2">
         <v>249.2907120441463</v>
@@ -426,7 +426,7 @@
         <v>84.54063340776146</v>
       </c>
       <c r="F2">
-        <v>2.58251337832879</v>
+        <v>1.848416664840239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Roadmap analysis. Mod8 modeling. Minor edits to Flux characterization
</commit_message>
<xml_diff>
--- a/Test_Data/1-23/results/Modeled power plot.xlsx
+++ b/Test_Data/1-23/results/Modeled power plot.xlsx
@@ -414,19 +414,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>16.52761147649603</v>
+        <v>13.53280827695495</v>
       </c>
       <c r="C2">
-        <v>66.80163065787728</v>
+        <v>54.69717518266992</v>
       </c>
       <c r="D2">
-        <v>249.2907120441463</v>
+        <v>204.119235021747</v>
       </c>
       <c r="E2">
-        <v>84.54063340776146</v>
+        <v>69.22187063427509</v>
       </c>
       <c r="F2">
-        <v>1.848416664840239</v>
+        <v>1.513483565171188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>